<commit_message>
add heavy augs with cutmix
</commit_message>
<xml_diff>
--- a/updates.xlsx
+++ b/updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Hungry/ML/Kaggle/Competition/cassava_/cassavana_kaggle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165E0AA6-74D9-CD4B-ABD8-5CED6D406566}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E8CE3D-576D-CC40-B3CE-8701FB17FCAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="28040" windowHeight="17440" xr2:uid="{A6265A70-2789-1444-8A69-A4166FAAE0FC}"/>
+    <workbookView xWindow="1500" yWindow="1320" windowWidth="21420" windowHeight="17440" xr2:uid="{A6265A70-2789-1444-8A69-A4166FAAE0FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -69,9 +69,6 @@
     <t>done</t>
   </si>
   <si>
-    <t xml:space="preserve"> + 4x tta and (randomcrop, flips transpose) </t>
-  </si>
-  <si>
     <t>cutmix variation</t>
   </si>
   <si>
@@ -81,25 +78,10 @@
     <t>no</t>
   </si>
   <si>
-    <t>Modification
- - Replace scheduler with ReduceOnPlateau 
- - Switch to 5fold instead of single fold</t>
-  </si>
-  <si>
     <t>Radam + Lookahead</t>
   </si>
   <si>
     <t>Bitempered loss/ Label smoothing loss/ Focal cosine loss</t>
-  </si>
-  <si>
-    <t>EffNet-B4 (baseline)
-- single fold (10 epoch)
-- noisystudent pretrained weights
-- cosineannealingwarmstart
-- simple augmentation (flips, crops, cutout)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - without tta</t>
   </si>
   <si>
     <t>Single model</t>
@@ -159,52 +141,27 @@
     <t>training with svm as 2nd stage</t>
   </si>
   <si>
-    <t>EffnetB4 + Vit_base16 (5fold ensemble + TTA w/o transpose)</t>
-  </si>
-  <si>
     <t>validation for ensemble</t>
   </si>
   <si>
     <t>**</t>
   </si>
   <si>
-    <t>w/o TTA</t>
-  </si>
-  <si>
-    <t>EffnetB4
+    <t>EffNet-B4 (baseline)
+- 5 fold (10 epoch)
 - cosineannealingwarmstart
-- randomcrop, hflip, vflip, transpose, cutout, 480
-- adam
-- single-fold</t>
-  </si>
-  <si>
-    <t>0.8848/0.8897</t>
-  </si>
-  <si>
-    <t>EffnetB4
+- simple augmentation (flips, crops, cutout, tranpose)
+ - Labelsmoothloss</t>
+  </si>
+  <si>
+    <t>EffNet-B4 (baseline)
+- 5 fold (10 epoch)
 - cosineannealingwarmstart
-- randomcrop, hflip, vflip, transpose, cutout, 512
-- adam
-- single-fold</t>
-  </si>
-  <si>
-    <t>0.884/0.893</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Vit_base_patch16
-- cosineannealingwarmstart
-- randomcrop, hflip, vflip, transpose, cutout, 384
-- adam
-- single-fold</t>
-  </si>
-  <si>
-    <t>0.881/0.889</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - labelsmoothing</t>
-  </si>
-  <si>
-    <t>0.891/0.892</t>
+- simple augmentation (flips, crops, cutout, tranpose)
+ - CE loss</t>
+  </si>
+  <si>
+    <t>0.884/0.891</t>
   </si>
 </sst>
 </file>
@@ -643,7 +600,7 @@
   <dimension ref="A2:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,19 +630,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.89</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.88400000000000001</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="H3" s="10" t="s">
         <v>8</v>
       </c>
@@ -693,17 +648,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="4">
-        <v>0.88800000000000001</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
@@ -711,20 +664,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="6"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="4">
-        <v>0.89800000000000002</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="2"/>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>5</v>
@@ -734,123 +680,80 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4">
-        <v>0.89300000000000002</v>
-      </c>
+      <c r="D6" s="4"/>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
       <c r="C7" s="15"/>
-      <c r="D7" s="4">
-        <v>0.90300000000000002</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
-        <v>0.90100000000000002</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>37</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="4"/>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>39</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>43</v>
-      </c>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="4"/>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>41</v>
-      </c>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="4"/>
       <c r="H12" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -871,17 +774,17 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H23" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>1</v>
@@ -890,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="H25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
@@ -898,19 +801,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C26" s="4">
         <v>0.876</v>
       </c>
       <c r="D26" s="4"/>
       <c r="H26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C27" s="4">
         <v>0.88600000000000001</v>
@@ -919,12 +822,12 @@
         <v>0.88500000000000001</v>
       </c>
       <c r="H27" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4">
         <v>0.88900000000000001</v>
@@ -935,7 +838,7 @@
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C29" s="4">
         <v>0.874</v>

</xml_diff>